<commit_message>
Bug fixes in exam module
</commit_message>
<xml_diff>
--- a/src/Static/files/MCQ.xlsx
+++ b/src/Static/files/MCQ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\projects\APR\src\Static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A432D300-9810-4ED3-9EA8-5CB2D638E456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5FB473-ED3F-476C-9333-E1428EB984A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FE00D8A4-64CB-4131-9480-31BEF3AB8A18}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t>E/M/H/D</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Explanation to why it's right</t>
   </si>
 </sst>
 </file>
@@ -421,18 +421,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8728EC-9B46-402B-A516-5D6D341A81D0}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.21875" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,8 +455,11 @@
       <c r="G1" t="s">
         <v>10</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -476,6 +480,9 @@
       </c>
       <c r="G2" t="s">
         <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>